<commit_message>
Revisons in Data Preparation
Indexes are ordered
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/ITC_Trade_Data/841810_UK_all.xlsx
+++ b/Data_Sources_and_Preparation/ITC_Trade_Data/841810_UK_all.xlsx
@@ -19,13 +19,13 @@
     <t>TUR_GBR_841810</t>
   </si>
   <si>
-    <t>KOR_GBR_841810</t>
+    <t>CHN_GBR_841810</t>
   </si>
   <si>
     <t>POL_GBR_841810</t>
   </si>
   <si>
-    <t>CHN_GBR_841810</t>
+    <t>KOR_GBR_841810</t>
   </si>
   <si>
     <t>ITA_GBR_841810</t>
@@ -871,11 +871,11 @@
       </c>
     </row>
     <row r="12" spans="1:31">
+      <c r="B12">
+        <v>1402</v>
+      </c>
       <c r="C12">
         <v>232</v>
-      </c>
-      <c r="D12">
-        <v>1402</v>
       </c>
       <c r="E12">
         <v>7813</v>
@@ -918,12 +918,12 @@
       <c r="A13">
         <v>52</v>
       </c>
+      <c r="B13">
+        <v>1009</v>
+      </c>
       <c r="C13">
         <v>457</v>
       </c>
-      <c r="D13">
-        <v>1009</v>
-      </c>
       <c r="E13">
         <v>8053</v>
       </c>
@@ -962,12 +962,12 @@
       </c>
     </row>
     <row r="14" spans="1:31">
+      <c r="B14">
+        <v>1216</v>
+      </c>
       <c r="C14">
         <v>159</v>
       </c>
-      <c r="D14">
-        <v>1216</v>
-      </c>
       <c r="E14">
         <v>7777</v>
       </c>
@@ -1018,11 +1018,11 @@
       </c>
     </row>
     <row r="15" spans="1:31">
+      <c r="B15">
+        <v>2042</v>
+      </c>
       <c r="C15">
         <v>366</v>
-      </c>
-      <c r="D15">
-        <v>2042</v>
       </c>
       <c r="E15">
         <v>6532</v>
@@ -1080,12 +1080,12 @@
       <c r="A16">
         <v>33</v>
       </c>
+      <c r="B16">
+        <v>2438</v>
+      </c>
       <c r="C16">
         <v>499</v>
       </c>
-      <c r="D16">
-        <v>2438</v>
-      </c>
       <c r="E16">
         <v>8923</v>
       </c>
@@ -1139,12 +1139,12 @@
       </c>
     </row>
     <row r="17" spans="1:31">
+      <c r="B17">
+        <v>2722</v>
+      </c>
       <c r="C17">
         <v>441</v>
       </c>
-      <c r="D17">
-        <v>2722</v>
-      </c>
       <c r="E17">
         <v>7674</v>
       </c>
@@ -1195,12 +1195,12 @@
       </c>
     </row>
     <row r="18" spans="1:31">
+      <c r="B18">
+        <v>2533</v>
+      </c>
       <c r="C18">
         <v>352</v>
       </c>
-      <c r="D18">
-        <v>2533</v>
-      </c>
       <c r="E18">
         <v>6431</v>
       </c>
@@ -1254,12 +1254,12 @@
       </c>
     </row>
     <row r="19" spans="1:31">
+      <c r="B19">
+        <v>4107</v>
+      </c>
       <c r="C19">
         <v>840</v>
       </c>
-      <c r="D19">
-        <v>4107</v>
-      </c>
       <c r="E19">
         <v>6038</v>
       </c>
@@ -1316,12 +1316,12 @@
       </c>
     </row>
     <row r="20" spans="1:31">
+      <c r="B20">
+        <v>3250</v>
+      </c>
       <c r="C20">
         <v>275</v>
       </c>
-      <c r="D20">
-        <v>3250</v>
-      </c>
       <c r="E20">
         <v>8907</v>
       </c>
@@ -1375,12 +1375,12 @@
       </c>
     </row>
     <row r="21" spans="1:31">
+      <c r="B21">
+        <v>2755</v>
+      </c>
       <c r="C21">
         <v>215</v>
       </c>
-      <c r="D21">
-        <v>2755</v>
-      </c>
       <c r="E21">
         <v>7662</v>
       </c>
@@ -1434,12 +1434,12 @@
       </c>
     </row>
     <row r="22" spans="1:31">
+      <c r="B22">
+        <v>3544</v>
+      </c>
       <c r="C22">
         <v>255</v>
       </c>
-      <c r="D22">
-        <v>3544</v>
-      </c>
       <c r="E22">
         <v>9529</v>
       </c>
@@ -1496,12 +1496,12 @@
       </c>
     </row>
     <row r="23" spans="1:31">
+      <c r="B23">
+        <v>2483</v>
+      </c>
       <c r="C23">
         <v>130</v>
       </c>
-      <c r="D23">
-        <v>2483</v>
-      </c>
       <c r="E23">
         <v>5823</v>
       </c>
@@ -1552,11 +1552,11 @@
       </c>
     </row>
     <row r="24" spans="1:31">
+      <c r="B24">
+        <v>2136</v>
+      </c>
       <c r="C24">
         <v>179</v>
-      </c>
-      <c r="D24">
-        <v>2136</v>
       </c>
       <c r="E24">
         <v>7106</v>
@@ -1614,12 +1614,12 @@
       <c r="A25">
         <v>5</v>
       </c>
+      <c r="B25">
+        <v>953</v>
+      </c>
       <c r="C25">
         <v>222</v>
       </c>
-      <c r="D25">
-        <v>953</v>
-      </c>
       <c r="E25">
         <v>4079</v>
       </c>
@@ -1676,12 +1676,12 @@
       </c>
     </row>
     <row r="26" spans="1:31">
+      <c r="B26">
+        <v>4079</v>
+      </c>
       <c r="C26">
         <v>169</v>
       </c>
-      <c r="D26">
-        <v>4079</v>
-      </c>
       <c r="E26">
         <v>8573</v>
       </c>
@@ -1738,12 +1738,12 @@
       </c>
     </row>
     <row r="27" spans="1:31">
+      <c r="B27">
+        <v>2323</v>
+      </c>
       <c r="C27">
         <v>250</v>
       </c>
-      <c r="D27">
-        <v>2323</v>
-      </c>
       <c r="E27">
         <v>6209</v>
       </c>
@@ -1800,11 +1800,11 @@
       </c>
     </row>
     <row r="28" spans="1:31">
+      <c r="B28">
+        <v>5824</v>
+      </c>
       <c r="C28">
         <v>277</v>
-      </c>
-      <c r="D28">
-        <v>5824</v>
       </c>
       <c r="E28">
         <v>8222</v>
@@ -1868,11 +1868,11 @@
       <c r="A29">
         <v>30</v>
       </c>
+      <c r="B29">
+        <v>7874</v>
+      </c>
       <c r="C29">
         <v>764</v>
-      </c>
-      <c r="D29">
-        <v>7874</v>
       </c>
       <c r="E29">
         <v>7312</v>
@@ -1930,11 +1930,11 @@
       <c r="A30">
         <v>10</v>
       </c>
+      <c r="B30">
+        <v>7287</v>
+      </c>
       <c r="C30">
         <v>366</v>
-      </c>
-      <c r="D30">
-        <v>7287</v>
       </c>
       <c r="E30">
         <v>9479</v>
@@ -1995,11 +1995,11 @@
       <c r="A31">
         <v>15</v>
       </c>
+      <c r="B31">
+        <v>14050</v>
+      </c>
       <c r="C31">
         <v>332</v>
-      </c>
-      <c r="D31">
-        <v>14050</v>
       </c>
       <c r="E31">
         <v>5914</v>
@@ -2066,11 +2066,11 @@
       <c r="A32">
         <v>93</v>
       </c>
+      <c r="B32">
+        <v>8070</v>
+      </c>
       <c r="C32">
         <v>244</v>
-      </c>
-      <c r="D32">
-        <v>8070</v>
       </c>
       <c r="E32">
         <v>9769</v>
@@ -2137,11 +2137,11 @@
       <c r="A33">
         <v>246</v>
       </c>
+      <c r="B33">
+        <v>12617</v>
+      </c>
       <c r="C33">
         <v>1556</v>
-      </c>
-      <c r="D33">
-        <v>12617</v>
       </c>
       <c r="E33">
         <v>11333</v>
@@ -2208,11 +2208,11 @@
       <c r="A34">
         <v>7548</v>
       </c>
+      <c r="B34">
+        <v>7766</v>
+      </c>
       <c r="C34">
         <v>446</v>
-      </c>
-      <c r="D34">
-        <v>7766</v>
       </c>
       <c r="E34">
         <v>9902</v>
@@ -2279,11 +2279,11 @@
       <c r="A35">
         <v>5796</v>
       </c>
+      <c r="B35">
+        <v>9841</v>
+      </c>
       <c r="C35">
         <v>676</v>
-      </c>
-      <c r="D35">
-        <v>9841</v>
       </c>
       <c r="E35">
         <v>5730</v>
@@ -2353,11 +2353,11 @@
       <c r="A36">
         <v>6397</v>
       </c>
+      <c r="B36">
+        <v>4094</v>
+      </c>
       <c r="C36">
         <v>1715</v>
-      </c>
-      <c r="D36">
-        <v>4094</v>
       </c>
       <c r="E36">
         <v>5842</v>
@@ -2427,11 +2427,11 @@
       <c r="A37">
         <v>6030</v>
       </c>
+      <c r="B37">
+        <v>7378</v>
+      </c>
       <c r="C37">
         <v>2219</v>
-      </c>
-      <c r="D37">
-        <v>7378</v>
       </c>
       <c r="E37">
         <v>7452</v>
@@ -2504,11 +2504,11 @@
       <c r="A38">
         <v>6373</v>
       </c>
+      <c r="B38">
+        <v>5818</v>
+      </c>
       <c r="C38">
         <v>770</v>
-      </c>
-      <c r="D38">
-        <v>5818</v>
       </c>
       <c r="E38">
         <v>5213</v>
@@ -2578,11 +2578,11 @@
       <c r="A39">
         <v>6893</v>
       </c>
+      <c r="B39">
+        <v>5785</v>
+      </c>
       <c r="C39">
         <v>278</v>
-      </c>
-      <c r="D39">
-        <v>5785</v>
       </c>
       <c r="E39">
         <v>6953</v>
@@ -2652,11 +2652,11 @@
       <c r="A40">
         <v>6122</v>
       </c>
+      <c r="B40">
+        <v>5587</v>
+      </c>
       <c r="C40">
         <v>359</v>
-      </c>
-      <c r="D40">
-        <v>5587</v>
       </c>
       <c r="E40">
         <v>9437</v>
@@ -2726,11 +2726,11 @@
       <c r="A41">
         <v>4507</v>
       </c>
+      <c r="B41">
+        <v>5617</v>
+      </c>
       <c r="C41">
         <v>808</v>
-      </c>
-      <c r="D41">
-        <v>5617</v>
       </c>
       <c r="E41">
         <v>7787</v>
@@ -2803,11 +2803,11 @@
       <c r="A42">
         <v>2382</v>
       </c>
+      <c r="B42">
+        <v>8591</v>
+      </c>
       <c r="C42">
         <v>2053</v>
-      </c>
-      <c r="D42">
-        <v>8591</v>
       </c>
       <c r="E42">
         <v>8372</v>
@@ -2880,11 +2880,11 @@
       <c r="A43">
         <v>3673</v>
       </c>
+      <c r="B43">
+        <v>11770</v>
+      </c>
       <c r="C43">
         <v>1180</v>
-      </c>
-      <c r="D43">
-        <v>11770</v>
       </c>
       <c r="E43">
         <v>5900</v>
@@ -2957,11 +2957,11 @@
       <c r="A44">
         <v>4907</v>
       </c>
+      <c r="B44">
+        <v>7401</v>
+      </c>
       <c r="C44">
         <v>2999</v>
-      </c>
-      <c r="D44">
-        <v>7401</v>
       </c>
       <c r="E44">
         <v>8136</v>
@@ -3034,11 +3034,11 @@
       <c r="A45">
         <v>6694</v>
       </c>
+      <c r="B45">
+        <v>6729</v>
+      </c>
       <c r="C45">
         <v>3797</v>
-      </c>
-      <c r="D45">
-        <v>6729</v>
       </c>
       <c r="E45">
         <v>10005</v>
@@ -3111,11 +3111,11 @@
       <c r="A46">
         <v>7148</v>
       </c>
+      <c r="B46">
+        <v>9328</v>
+      </c>
       <c r="C46">
         <v>3450</v>
-      </c>
-      <c r="D46">
-        <v>9328</v>
       </c>
       <c r="E46">
         <v>6543</v>
@@ -3188,11 +3188,11 @@
       <c r="A47">
         <v>4496</v>
       </c>
+      <c r="B47">
+        <v>5935</v>
+      </c>
       <c r="C47">
         <v>2873</v>
-      </c>
-      <c r="D47">
-        <v>5935</v>
       </c>
       <c r="E47">
         <v>4002</v>
@@ -3266,13 +3266,13 @@
         <v>2687</v>
       </c>
       <c r="B48">
-        <v>9720</v>
+        <v>2707</v>
       </c>
       <c r="C48">
         <v>2102</v>
       </c>
       <c r="D48">
-        <v>2707</v>
+        <v>9720</v>
       </c>
       <c r="E48">
         <v>6626</v>
@@ -3346,13 +3346,13 @@
         <v>3498</v>
       </c>
       <c r="B49">
-        <v>3528</v>
+        <v>2860</v>
       </c>
       <c r="C49">
         <v>1124</v>
       </c>
       <c r="D49">
-        <v>2860</v>
+        <v>3528</v>
       </c>
       <c r="E49">
         <v>7403</v>
@@ -3429,13 +3429,13 @@
         <v>2666</v>
       </c>
       <c r="B50">
-        <v>2950</v>
+        <v>3738</v>
       </c>
       <c r="C50">
         <v>1317</v>
       </c>
       <c r="D50">
-        <v>3738</v>
+        <v>2950</v>
       </c>
       <c r="E50">
         <v>8205</v>
@@ -3515,13 +3515,13 @@
         <v>2974</v>
       </c>
       <c r="B51">
-        <v>2566</v>
+        <v>5306</v>
       </c>
       <c r="C51">
         <v>1993</v>
       </c>
       <c r="D51">
-        <v>5306</v>
+        <v>2566</v>
       </c>
       <c r="E51">
         <v>7009</v>
@@ -3604,13 +3604,13 @@
         <v>3612</v>
       </c>
       <c r="B52">
-        <v>2844</v>
+        <v>6653</v>
       </c>
       <c r="C52">
         <v>996</v>
       </c>
       <c r="D52">
-        <v>6653</v>
+        <v>2844</v>
       </c>
       <c r="E52">
         <v>5753</v>
@@ -3693,13 +3693,13 @@
         <v>3973</v>
       </c>
       <c r="B53">
-        <v>2502</v>
+        <v>7005</v>
       </c>
       <c r="C53">
         <v>662</v>
       </c>
       <c r="D53">
-        <v>7005</v>
+        <v>2502</v>
       </c>
       <c r="E53">
         <v>6553</v>
@@ -3782,13 +3782,13 @@
         <v>5747</v>
       </c>
       <c r="B54">
-        <v>4566</v>
+        <v>11231</v>
       </c>
       <c r="C54">
         <v>1022</v>
       </c>
       <c r="D54">
-        <v>11231</v>
+        <v>4566</v>
       </c>
       <c r="E54">
         <v>7758</v>
@@ -3874,13 +3874,13 @@
         <v>5511</v>
       </c>
       <c r="B55">
-        <v>6592</v>
+        <v>7539</v>
       </c>
       <c r="C55">
         <v>1699</v>
       </c>
       <c r="D55">
-        <v>7539</v>
+        <v>6592</v>
       </c>
       <c r="E55">
         <v>2456</v>
@@ -3966,13 +3966,13 @@
         <v>5468</v>
       </c>
       <c r="B56">
-        <v>2227</v>
+        <v>6107</v>
       </c>
       <c r="C56">
         <v>1382</v>
       </c>
       <c r="D56">
-        <v>6107</v>
+        <v>2227</v>
       </c>
       <c r="E56">
         <v>5210</v>
@@ -4058,13 +4058,13 @@
         <v>4048</v>
       </c>
       <c r="B57">
-        <v>7400</v>
+        <v>5892</v>
       </c>
       <c r="C57">
         <v>794</v>
       </c>
       <c r="D57">
-        <v>5892</v>
+        <v>7400</v>
       </c>
       <c r="E57">
         <v>4389</v>
@@ -4150,13 +4150,13 @@
         <v>3860</v>
       </c>
       <c r="B58">
-        <v>2501</v>
+        <v>7033</v>
       </c>
       <c r="C58">
         <v>101</v>
       </c>
       <c r="D58">
-        <v>7033</v>
+        <v>2501</v>
       </c>
       <c r="E58">
         <v>3746</v>
@@ -4242,13 +4242,13 @@
         <v>3381</v>
       </c>
       <c r="B59">
-        <v>2287</v>
+        <v>3566</v>
       </c>
       <c r="C59">
         <v>989</v>
       </c>
       <c r="D59">
-        <v>3566</v>
+        <v>2287</v>
       </c>
       <c r="E59">
         <v>2706</v>
@@ -4334,13 +4334,13 @@
         <v>1945</v>
       </c>
       <c r="B60">
-        <v>1172</v>
+        <v>3057</v>
       </c>
       <c r="C60">
         <v>506</v>
       </c>
       <c r="D60">
-        <v>3057</v>
+        <v>1172</v>
       </c>
       <c r="E60">
         <v>2345</v>
@@ -4429,13 +4429,13 @@
         <v>1240</v>
       </c>
       <c r="B61">
-        <v>3153</v>
+        <v>1759</v>
       </c>
       <c r="C61">
         <v>320</v>
       </c>
       <c r="D61">
-        <v>1759</v>
+        <v>3153</v>
       </c>
       <c r="E61">
         <v>3010</v>
@@ -4524,13 +4524,13 @@
         <v>4215</v>
       </c>
       <c r="B62">
-        <v>3729</v>
+        <v>4468</v>
       </c>
       <c r="C62">
         <v>1106</v>
       </c>
       <c r="D62">
-        <v>4468</v>
+        <v>3729</v>
       </c>
       <c r="E62">
         <v>2769</v>
@@ -4619,13 +4619,13 @@
         <v>4060</v>
       </c>
       <c r="B63">
-        <v>4255</v>
+        <v>3991</v>
       </c>
       <c r="C63">
         <v>1124</v>
       </c>
       <c r="D63">
-        <v>3991</v>
+        <v>4255</v>
       </c>
       <c r="E63">
         <v>2339</v>
@@ -4714,13 +4714,13 @@
         <v>3808</v>
       </c>
       <c r="B64">
-        <v>5835</v>
+        <v>3900</v>
       </c>
       <c r="C64">
         <v>1118</v>
       </c>
       <c r="D64">
-        <v>3900</v>
+        <v>5835</v>
       </c>
       <c r="E64">
         <v>4350</v>
@@ -4809,13 +4809,13 @@
         <v>5951</v>
       </c>
       <c r="B65">
-        <v>6258</v>
+        <v>6669</v>
       </c>
       <c r="C65">
         <v>1676</v>
       </c>
       <c r="D65">
-        <v>6669</v>
+        <v>6258</v>
       </c>
       <c r="E65">
         <v>3673</v>
@@ -4904,13 +4904,13 @@
         <v>6497</v>
       </c>
       <c r="B66">
-        <v>7732</v>
+        <v>7989</v>
       </c>
       <c r="C66">
         <v>1315</v>
       </c>
       <c r="D66">
-        <v>7989</v>
+        <v>7732</v>
       </c>
       <c r="E66">
         <v>2526</v>
@@ -4999,13 +4999,13 @@
         <v>4371</v>
       </c>
       <c r="B67">
-        <v>8170</v>
+        <v>5423</v>
       </c>
       <c r="C67">
         <v>1549</v>
       </c>
       <c r="D67">
-        <v>5423</v>
+        <v>8170</v>
       </c>
       <c r="E67">
         <v>1851</v>
@@ -5094,13 +5094,13 @@
         <v>6024</v>
       </c>
       <c r="B68">
-        <v>7814</v>
+        <v>5094</v>
       </c>
       <c r="C68">
         <v>1753</v>
       </c>
       <c r="D68">
-        <v>5094</v>
+        <v>7814</v>
       </c>
       <c r="E68">
         <v>2623</v>
@@ -5189,13 +5189,13 @@
         <v>4764</v>
       </c>
       <c r="B69">
-        <v>6326</v>
+        <v>4843</v>
       </c>
       <c r="C69">
         <v>1120</v>
       </c>
       <c r="D69">
-        <v>4843</v>
+        <v>6326</v>
       </c>
       <c r="E69">
         <v>2731</v>
@@ -5284,13 +5284,13 @@
         <v>5872</v>
       </c>
       <c r="B70">
-        <v>6816</v>
+        <v>6179</v>
       </c>
       <c r="C70">
         <v>1700</v>
       </c>
       <c r="D70">
-        <v>6179</v>
+        <v>6816</v>
       </c>
       <c r="E70">
         <v>2958</v>
@@ -5379,13 +5379,13 @@
         <v>5365</v>
       </c>
       <c r="B71">
-        <v>6937</v>
+        <v>5671</v>
       </c>
       <c r="C71">
         <v>1991</v>
       </c>
       <c r="D71">
-        <v>5671</v>
+        <v>6937</v>
       </c>
       <c r="E71">
         <v>2036</v>
@@ -5474,13 +5474,13 @@
         <v>4151</v>
       </c>
       <c r="B72">
-        <v>7796</v>
+        <v>6630</v>
       </c>
       <c r="C72">
         <v>1379</v>
       </c>
       <c r="D72">
-        <v>6630</v>
+        <v>7796</v>
       </c>
       <c r="E72">
         <v>2552</v>
@@ -5569,13 +5569,13 @@
         <v>4619</v>
       </c>
       <c r="B73">
-        <v>4881</v>
+        <v>3596</v>
       </c>
       <c r="C73">
         <v>1405</v>
       </c>
       <c r="D73">
-        <v>3596</v>
+        <v>4881</v>
       </c>
       <c r="E73">
         <v>2263</v>
@@ -5664,13 +5664,13 @@
         <v>2964</v>
       </c>
       <c r="B74">
-        <v>5086</v>
+        <v>5305</v>
       </c>
       <c r="C74">
         <v>780</v>
       </c>
       <c r="D74">
-        <v>5305</v>
+        <v>5086</v>
       </c>
       <c r="E74">
         <v>2645</v>
@@ -5759,13 +5759,13 @@
         <v>3755</v>
       </c>
       <c r="B75">
-        <v>4821</v>
+        <v>4570</v>
       </c>
       <c r="C75">
         <v>876</v>
       </c>
       <c r="D75">
-        <v>4570</v>
+        <v>4821</v>
       </c>
       <c r="E75">
         <v>1904</v>
@@ -5854,13 +5854,13 @@
         <v>2788</v>
       </c>
       <c r="B76">
-        <v>4504</v>
+        <v>6012</v>
       </c>
       <c r="C76">
         <v>1231</v>
       </c>
       <c r="D76">
-        <v>6012</v>
+        <v>4504</v>
       </c>
       <c r="E76">
         <v>1910</v>
@@ -5949,13 +5949,13 @@
         <v>3647</v>
       </c>
       <c r="B77">
-        <v>4016</v>
+        <v>7574</v>
       </c>
       <c r="C77">
         <v>840</v>
       </c>
       <c r="D77">
-        <v>7574</v>
+        <v>4016</v>
       </c>
       <c r="E77">
         <v>1616</v>
@@ -6044,13 +6044,13 @@
         <v>4301</v>
       </c>
       <c r="B78">
-        <v>5199</v>
+        <v>8714</v>
       </c>
       <c r="C78">
         <v>1383</v>
       </c>
       <c r="D78">
-        <v>8714</v>
+        <v>5199</v>
       </c>
       <c r="E78">
         <v>2676</v>
@@ -6139,13 +6139,13 @@
         <v>6466</v>
       </c>
       <c r="B79">
-        <v>3271</v>
+        <v>7438</v>
       </c>
       <c r="C79">
         <v>1009</v>
       </c>
       <c r="D79">
-        <v>7438</v>
+        <v>3271</v>
       </c>
       <c r="E79">
         <v>1130</v>
@@ -6234,13 +6234,13 @@
         <v>3939</v>
       </c>
       <c r="B80">
-        <v>4399</v>
+        <v>12109</v>
       </c>
       <c r="C80">
         <v>1386</v>
       </c>
       <c r="D80">
-        <v>12109</v>
+        <v>4399</v>
       </c>
       <c r="E80">
         <v>2263</v>
@@ -6329,13 +6329,13 @@
         <v>6680</v>
       </c>
       <c r="B81">
-        <v>9423</v>
+        <v>11300</v>
       </c>
       <c r="C81">
         <v>1706</v>
       </c>
       <c r="D81">
-        <v>11300</v>
+        <v>9423</v>
       </c>
       <c r="E81">
         <v>2011</v>
@@ -6424,13 +6424,13 @@
         <v>6980</v>
       </c>
       <c r="B82">
-        <v>10004</v>
+        <v>13699</v>
       </c>
       <c r="C82">
         <v>1810</v>
       </c>
       <c r="D82">
-        <v>13699</v>
+        <v>10004</v>
       </c>
       <c r="E82">
         <v>1991</v>
@@ -6519,13 +6519,13 @@
         <v>8866</v>
       </c>
       <c r="B83">
-        <v>5388</v>
+        <v>9113</v>
       </c>
       <c r="C83">
         <v>2570</v>
       </c>
       <c r="D83">
-        <v>9113</v>
+        <v>5388</v>
       </c>
       <c r="E83">
         <v>1566</v>
@@ -6614,13 +6614,13 @@
         <v>3666</v>
       </c>
       <c r="B84">
-        <v>3645</v>
+        <v>5961</v>
       </c>
       <c r="C84">
         <v>1415</v>
       </c>
       <c r="D84">
-        <v>5961</v>
+        <v>3645</v>
       </c>
       <c r="E84">
         <v>2112</v>
@@ -6709,13 +6709,13 @@
         <v>4200</v>
       </c>
       <c r="B85">
-        <v>4686</v>
+        <v>4020</v>
       </c>
       <c r="C85">
         <v>2204</v>
       </c>
       <c r="D85">
-        <v>4020</v>
+        <v>4686</v>
       </c>
       <c r="E85">
         <v>2331</v>
@@ -6804,13 +6804,13 @@
         <v>4676</v>
       </c>
       <c r="B86">
-        <v>4514</v>
+        <v>5855</v>
       </c>
       <c r="C86">
         <v>2546</v>
       </c>
       <c r="D86">
-        <v>5855</v>
+        <v>4514</v>
       </c>
       <c r="E86">
         <v>2990</v>
@@ -6899,13 +6899,13 @@
         <v>6860</v>
       </c>
       <c r="B87">
-        <v>3868</v>
+        <v>5534</v>
       </c>
       <c r="C87">
         <v>2397</v>
       </c>
       <c r="D87">
-        <v>5534</v>
+        <v>3868</v>
       </c>
       <c r="E87">
         <v>2263</v>
@@ -6994,13 +6994,13 @@
         <v>6964</v>
       </c>
       <c r="B88">
-        <v>4292</v>
+        <v>6855</v>
       </c>
       <c r="C88">
         <v>2586</v>
       </c>
       <c r="D88">
-        <v>6855</v>
+        <v>4292</v>
       </c>
       <c r="E88">
         <v>2730</v>
@@ -7089,13 +7089,13 @@
         <v>8309</v>
       </c>
       <c r="B89">
-        <v>3140</v>
+        <v>8636</v>
       </c>
       <c r="C89">
         <v>3186</v>
       </c>
       <c r="D89">
-        <v>8636</v>
+        <v>3140</v>
       </c>
       <c r="E89">
         <v>2348</v>
@@ -7184,13 +7184,13 @@
         <v>7117</v>
       </c>
       <c r="B90">
-        <v>2360</v>
+        <v>7769</v>
       </c>
       <c r="C90">
         <v>2196</v>
       </c>
       <c r="D90">
-        <v>7769</v>
+        <v>2360</v>
       </c>
       <c r="E90">
         <v>2095</v>
@@ -7279,13 +7279,13 @@
         <v>11812</v>
       </c>
       <c r="B91">
-        <v>3350</v>
+        <v>5226</v>
       </c>
       <c r="C91">
         <v>2650</v>
       </c>
       <c r="D91">
-        <v>5226</v>
+        <v>3350</v>
       </c>
       <c r="E91">
         <v>1631</v>
@@ -7374,13 +7374,13 @@
         <v>11039</v>
       </c>
       <c r="B92">
-        <v>6064</v>
+        <v>6190</v>
       </c>
       <c r="C92">
         <v>2738</v>
       </c>
       <c r="D92">
-        <v>6190</v>
+        <v>6064</v>
       </c>
       <c r="E92">
         <v>2890</v>
@@ -7469,13 +7469,13 @@
         <v>15952</v>
       </c>
       <c r="B93">
-        <v>8203</v>
+        <v>6966</v>
       </c>
       <c r="C93">
         <v>2879</v>
       </c>
       <c r="D93">
-        <v>6966</v>
+        <v>8203</v>
       </c>
       <c r="E93">
         <v>2829</v>
@@ -7564,13 +7564,13 @@
         <v>16062</v>
       </c>
       <c r="B94">
-        <v>5503</v>
+        <v>6447</v>
       </c>
       <c r="C94">
         <v>4500</v>
       </c>
       <c r="D94">
-        <v>6447</v>
+        <v>5503</v>
       </c>
       <c r="E94">
         <v>2465</v>
@@ -7659,13 +7659,13 @@
         <v>15322</v>
       </c>
       <c r="B95">
-        <v>3497</v>
+        <v>7746</v>
       </c>
       <c r="C95">
         <v>2921</v>
       </c>
       <c r="D95">
-        <v>7746</v>
+        <v>3497</v>
       </c>
       <c r="E95">
         <v>1744</v>
@@ -7754,13 +7754,13 @@
         <v>10179</v>
       </c>
       <c r="B96">
-        <v>3923</v>
+        <v>7427</v>
       </c>
       <c r="C96">
         <v>2472</v>
       </c>
       <c r="D96">
-        <v>7427</v>
+        <v>3923</v>
       </c>
       <c r="E96">
         <v>2271</v>
@@ -7849,13 +7849,13 @@
         <v>9516</v>
       </c>
       <c r="B97">
-        <v>3086</v>
+        <v>4169</v>
       </c>
       <c r="C97">
         <v>1609</v>
       </c>
       <c r="D97">
-        <v>4169</v>
+        <v>3086</v>
       </c>
       <c r="E97">
         <v>2189</v>
@@ -7944,13 +7944,13 @@
         <v>13462</v>
       </c>
       <c r="B98">
-        <v>2258</v>
+        <v>6163</v>
       </c>
       <c r="C98">
         <v>1512</v>
       </c>
       <c r="D98">
-        <v>6163</v>
+        <v>2258</v>
       </c>
       <c r="E98">
         <v>2595</v>
@@ -8039,13 +8039,13 @@
         <v>13930</v>
       </c>
       <c r="B99">
-        <v>3800</v>
+        <v>12703</v>
       </c>
       <c r="C99">
         <v>564</v>
       </c>
       <c r="D99">
-        <v>12703</v>
+        <v>3800</v>
       </c>
       <c r="E99">
         <v>2853</v>
@@ -8134,13 +8134,13 @@
         <v>12476</v>
       </c>
       <c r="B100">
-        <v>4544</v>
+        <v>15469</v>
       </c>
       <c r="C100">
         <v>2380</v>
       </c>
       <c r="D100">
-        <v>15469</v>
+        <v>4544</v>
       </c>
       <c r="E100">
         <v>2449</v>
@@ -8229,13 +8229,13 @@
         <v>17163</v>
       </c>
       <c r="B101">
-        <v>3559</v>
+        <v>16733</v>
       </c>
       <c r="C101">
         <v>2345</v>
       </c>
       <c r="D101">
-        <v>16733</v>
+        <v>3559</v>
       </c>
       <c r="E101">
         <v>2399</v>
@@ -8324,13 +8324,13 @@
         <v>12094</v>
       </c>
       <c r="B102">
-        <v>4189</v>
+        <v>14717</v>
       </c>
       <c r="C102">
         <v>3003</v>
       </c>
       <c r="D102">
-        <v>14717</v>
+        <v>4189</v>
       </c>
       <c r="E102">
         <v>2012</v>
@@ -8419,13 +8419,13 @@
         <v>14484</v>
       </c>
       <c r="B103">
-        <v>3987</v>
+        <v>12200</v>
       </c>
       <c r="C103">
         <v>4506</v>
       </c>
       <c r="D103">
-        <v>12200</v>
+        <v>3987</v>
       </c>
       <c r="E103">
         <v>1383</v>
@@ -8514,13 +8514,13 @@
         <v>13848</v>
       </c>
       <c r="B104">
-        <v>5094</v>
+        <v>14356</v>
       </c>
       <c r="C104">
         <v>5548</v>
       </c>
       <c r="D104">
-        <v>14356</v>
+        <v>5094</v>
       </c>
       <c r="E104">
         <v>2740</v>
@@ -8609,13 +8609,13 @@
         <v>16337</v>
       </c>
       <c r="B105">
-        <v>7045</v>
+        <v>15549</v>
       </c>
       <c r="C105">
         <v>6049</v>
       </c>
       <c r="D105">
-        <v>15549</v>
+        <v>7045</v>
       </c>
       <c r="E105">
         <v>2704</v>
@@ -8704,13 +8704,13 @@
         <v>10824</v>
       </c>
       <c r="B106">
-        <v>3215</v>
+        <v>13952</v>
       </c>
       <c r="C106">
         <v>4651</v>
       </c>
       <c r="D106">
-        <v>13952</v>
+        <v>3215</v>
       </c>
       <c r="E106">
         <v>2841</v>
@@ -8799,13 +8799,13 @@
         <v>12786</v>
       </c>
       <c r="B107">
-        <v>2778</v>
+        <v>14077</v>
       </c>
       <c r="C107">
         <v>3306</v>
       </c>
       <c r="D107">
-        <v>14077</v>
+        <v>2778</v>
       </c>
       <c r="E107">
         <v>2178</v>
@@ -8894,13 +8894,13 @@
         <v>12447</v>
       </c>
       <c r="B108">
-        <v>3098</v>
+        <v>7997</v>
       </c>
       <c r="C108">
         <v>3328</v>
       </c>
       <c r="D108">
-        <v>7997</v>
+        <v>3098</v>
       </c>
       <c r="E108">
         <v>2327</v>
@@ -8989,13 +8989,13 @@
         <v>12877</v>
       </c>
       <c r="B109">
-        <v>2072</v>
+        <v>6428</v>
       </c>
       <c r="C109">
         <v>2524</v>
       </c>
       <c r="D109">
-        <v>6428</v>
+        <v>2072</v>
       </c>
       <c r="E109">
         <v>2649</v>
@@ -9084,13 +9084,13 @@
         <v>9519</v>
       </c>
       <c r="B110">
-        <v>2364</v>
+        <v>10348</v>
       </c>
       <c r="C110">
         <v>4262</v>
       </c>
       <c r="D110">
-        <v>10348</v>
+        <v>2364</v>
       </c>
       <c r="E110">
         <v>2234</v>
@@ -9179,13 +9179,13 @@
         <v>10131</v>
       </c>
       <c r="B111">
-        <v>2285</v>
+        <v>10959</v>
       </c>
       <c r="C111">
         <v>4656</v>
       </c>
       <c r="D111">
-        <v>10959</v>
+        <v>2285</v>
       </c>
       <c r="E111">
         <v>2120</v>
@@ -9274,13 +9274,13 @@
         <v>7622</v>
       </c>
       <c r="B112">
-        <v>4987</v>
+        <v>13744</v>
       </c>
       <c r="C112">
         <v>4409</v>
       </c>
       <c r="D112">
-        <v>13744</v>
+        <v>4987</v>
       </c>
       <c r="E112">
         <v>2629</v>
@@ -9369,13 +9369,13 @@
         <v>9936</v>
       </c>
       <c r="B113">
-        <v>4260</v>
+        <v>13248</v>
       </c>
       <c r="C113">
         <v>8031</v>
       </c>
       <c r="D113">
-        <v>13248</v>
+        <v>4260</v>
       </c>
       <c r="E113">
         <v>1951</v>
@@ -9464,13 +9464,13 @@
         <v>14855</v>
       </c>
       <c r="B114">
-        <v>3816</v>
+        <v>15548</v>
       </c>
       <c r="C114">
         <v>5278</v>
       </c>
       <c r="D114">
-        <v>15548</v>
+        <v>3816</v>
       </c>
       <c r="E114">
         <v>2656</v>
@@ -9559,13 +9559,13 @@
         <v>12125</v>
       </c>
       <c r="B115">
-        <v>3431</v>
+        <v>12820</v>
       </c>
       <c r="C115">
         <v>6641</v>
       </c>
       <c r="D115">
-        <v>12820</v>
+        <v>3431</v>
       </c>
       <c r="E115">
         <v>1842</v>
@@ -9654,13 +9654,13 @@
         <v>20206</v>
       </c>
       <c r="B116">
-        <v>6406</v>
+        <v>8230</v>
       </c>
       <c r="C116">
         <v>6837</v>
       </c>
       <c r="D116">
-        <v>8230</v>
+        <v>6406</v>
       </c>
       <c r="E116">
         <v>3714</v>
@@ -9749,13 +9749,13 @@
         <v>18742</v>
       </c>
       <c r="B117">
-        <v>8204</v>
+        <v>7677</v>
       </c>
       <c r="C117">
         <v>7328</v>
       </c>
       <c r="D117">
-        <v>7677</v>
+        <v>8204</v>
       </c>
       <c r="E117">
         <v>3387</v>
@@ -9844,13 +9844,13 @@
         <v>12429</v>
       </c>
       <c r="B118">
-        <v>2351</v>
+        <v>8184</v>
       </c>
       <c r="C118">
         <v>4978</v>
       </c>
       <c r="D118">
-        <v>8184</v>
+        <v>2351</v>
       </c>
       <c r="E118">
         <v>2007</v>
@@ -9939,13 +9939,13 @@
         <v>13422</v>
       </c>
       <c r="B119">
-        <v>2368</v>
+        <v>7228</v>
       </c>
       <c r="C119">
         <v>5489</v>
       </c>
       <c r="D119">
-        <v>7228</v>
+        <v>2368</v>
       </c>
       <c r="E119">
         <v>1360</v>
@@ -10034,13 +10034,13 @@
         <v>9674</v>
       </c>
       <c r="B120">
-        <v>3991</v>
+        <v>6569</v>
       </c>
       <c r="C120">
         <v>6099</v>
       </c>
       <c r="D120">
-        <v>6569</v>
+        <v>3991</v>
       </c>
       <c r="E120">
         <v>2249</v>
@@ -10129,13 +10129,13 @@
         <v>9354</v>
       </c>
       <c r="B121">
-        <v>2601</v>
+        <v>5185</v>
       </c>
       <c r="C121">
         <v>4587</v>
       </c>
       <c r="D121">
-        <v>5185</v>
+        <v>2601</v>
       </c>
       <c r="E121">
         <v>1573</v>
@@ -10224,13 +10224,13 @@
         <v>11246</v>
       </c>
       <c r="B122">
-        <v>4089</v>
+        <v>7955</v>
       </c>
       <c r="C122">
         <v>4168</v>
       </c>
       <c r="D122">
-        <v>7955</v>
+        <v>4089</v>
       </c>
       <c r="E122">
         <v>3621</v>
@@ -10319,13 +10319,13 @@
         <v>13577</v>
       </c>
       <c r="B123">
-        <v>2957</v>
+        <v>16958</v>
       </c>
       <c r="C123">
         <v>4447</v>
       </c>
       <c r="D123">
-        <v>16958</v>
+        <v>2957</v>
       </c>
       <c r="E123">
         <v>2381</v>
@@ -10414,13 +10414,13 @@
         <v>11427</v>
       </c>
       <c r="B124">
-        <v>5321</v>
+        <v>11482</v>
       </c>
       <c r="C124">
         <v>6139</v>
       </c>
       <c r="D124">
-        <v>11482</v>
+        <v>5321</v>
       </c>
       <c r="E124">
         <v>2676</v>
@@ -10509,13 +10509,13 @@
         <v>16536</v>
       </c>
       <c r="B125">
-        <v>6973</v>
+        <v>20962</v>
       </c>
       <c r="C125">
         <v>8550</v>
       </c>
       <c r="D125">
-        <v>20962</v>
+        <v>6973</v>
       </c>
       <c r="E125">
         <v>2787</v>
@@ -10604,13 +10604,13 @@
         <v>18120</v>
       </c>
       <c r="B126">
-        <v>6059</v>
+        <v>14071</v>
       </c>
       <c r="C126">
         <v>5759</v>
       </c>
       <c r="D126">
-        <v>14071</v>
+        <v>6059</v>
       </c>
       <c r="E126">
         <v>2505</v>
@@ -10699,13 +10699,13 @@
         <v>14919</v>
       </c>
       <c r="B127">
-        <v>4395</v>
+        <v>16613</v>
       </c>
       <c r="C127">
         <v>8110</v>
       </c>
       <c r="D127">
-        <v>16613</v>
+        <v>4395</v>
       </c>
       <c r="E127">
         <v>1716</v>
@@ -10794,13 +10794,13 @@
         <v>17789</v>
       </c>
       <c r="B128">
-        <v>5982</v>
+        <v>16420</v>
       </c>
       <c r="C128">
         <v>5007</v>
       </c>
       <c r="D128">
-        <v>16420</v>
+        <v>5982</v>
       </c>
       <c r="E128">
         <v>3354</v>
@@ -10889,13 +10889,13 @@
         <v>13338</v>
       </c>
       <c r="B129">
-        <v>5705</v>
+        <v>11025</v>
       </c>
       <c r="C129">
         <v>6430</v>
       </c>
       <c r="D129">
-        <v>11025</v>
+        <v>5705</v>
       </c>
       <c r="E129">
         <v>3583</v>
@@ -10984,13 +10984,13 @@
         <v>11807</v>
       </c>
       <c r="B130">
-        <v>3927</v>
+        <v>9787</v>
       </c>
       <c r="C130">
         <v>6313</v>
       </c>
       <c r="D130">
-        <v>9787</v>
+        <v>3927</v>
       </c>
       <c r="E130">
         <v>3568</v>
@@ -11079,13 +11079,13 @@
         <v>9400</v>
       </c>
       <c r="B131">
-        <v>3751</v>
+        <v>10012</v>
       </c>
       <c r="C131">
         <v>6136</v>
       </c>
       <c r="D131">
-        <v>10012</v>
+        <v>3751</v>
       </c>
       <c r="E131">
         <v>1977</v>
@@ -11174,13 +11174,13 @@
         <v>7199</v>
       </c>
       <c r="B132">
-        <v>3338</v>
+        <v>11755</v>
       </c>
       <c r="C132">
         <v>4149</v>
       </c>
       <c r="D132">
-        <v>11755</v>
+        <v>3338</v>
       </c>
       <c r="E132">
         <v>3294</v>
@@ -11269,13 +11269,13 @@
         <v>7518</v>
       </c>
       <c r="B133">
-        <v>2154</v>
+        <v>9766</v>
       </c>
       <c r="C133">
         <v>2546</v>
       </c>
       <c r="D133">
-        <v>9766</v>
+        <v>2154</v>
       </c>
       <c r="E133">
         <v>3681</v>
@@ -11364,13 +11364,13 @@
         <v>8651</v>
       </c>
       <c r="B134">
-        <v>4347</v>
+        <v>10431</v>
       </c>
       <c r="C134">
         <v>4227</v>
       </c>
       <c r="D134">
-        <v>10431</v>
+        <v>4347</v>
       </c>
       <c r="E134">
         <v>2751</v>
@@ -11459,13 +11459,13 @@
         <v>10365</v>
       </c>
       <c r="B135">
-        <v>4386</v>
+        <v>9058</v>
       </c>
       <c r="C135">
         <v>3684</v>
       </c>
       <c r="D135">
-        <v>9058</v>
+        <v>4386</v>
       </c>
       <c r="E135">
         <v>3224</v>
@@ -11554,13 +11554,13 @@
         <v>7802</v>
       </c>
       <c r="B136">
-        <v>2541</v>
+        <v>11683</v>
       </c>
       <c r="C136">
         <v>3166</v>
       </c>
       <c r="D136">
-        <v>11683</v>
+        <v>2541</v>
       </c>
       <c r="E136">
         <v>3849</v>
@@ -11649,13 +11649,13 @@
         <v>12593</v>
       </c>
       <c r="B137">
-        <v>2259</v>
+        <v>8536</v>
       </c>
       <c r="C137">
         <v>6225</v>
       </c>
       <c r="D137">
-        <v>8536</v>
+        <v>2259</v>
       </c>
       <c r="E137">
         <v>3862</v>
@@ -11744,13 +11744,13 @@
         <v>11406</v>
       </c>
       <c r="B138">
-        <v>4830</v>
+        <v>8920</v>
       </c>
       <c r="C138">
         <v>6006</v>
       </c>
       <c r="D138">
-        <v>8920</v>
+        <v>4830</v>
       </c>
       <c r="E138">
         <v>3732</v>
@@ -11839,13 +11839,13 @@
         <v>10671</v>
       </c>
       <c r="B139">
-        <v>2325</v>
+        <v>14194</v>
       </c>
       <c r="C139">
         <v>5909</v>
       </c>
       <c r="D139">
-        <v>14194</v>
+        <v>2325</v>
       </c>
       <c r="E139">
         <v>2621</v>
@@ -11934,13 +11934,13 @@
         <v>13414</v>
       </c>
       <c r="B140">
-        <v>4447</v>
+        <v>10988</v>
       </c>
       <c r="C140">
         <v>6343</v>
       </c>
       <c r="D140">
-        <v>10988</v>
+        <v>4447</v>
       </c>
       <c r="E140">
         <v>4735</v>
@@ -12029,13 +12029,13 @@
         <v>12048</v>
       </c>
       <c r="B141">
-        <v>5812</v>
+        <v>11724</v>
       </c>
       <c r="C141">
         <v>7651</v>
       </c>
       <c r="D141">
-        <v>11724</v>
+        <v>5812</v>
       </c>
       <c r="E141">
         <v>5730</v>
@@ -12124,13 +12124,13 @@
         <v>13764</v>
       </c>
       <c r="B142">
-        <v>3621</v>
+        <v>8194</v>
       </c>
       <c r="C142">
         <v>6196</v>
       </c>
       <c r="D142">
-        <v>8194</v>
+        <v>3621</v>
       </c>
       <c r="E142">
         <v>4180</v>
@@ -12219,13 +12219,13 @@
         <v>10207</v>
       </c>
       <c r="B143">
-        <v>1957</v>
+        <v>9131</v>
       </c>
       <c r="C143">
         <v>4852</v>
       </c>
       <c r="D143">
-        <v>9131</v>
+        <v>1957</v>
       </c>
       <c r="E143">
         <v>2475</v>
@@ -12314,13 +12314,13 @@
         <v>7440</v>
       </c>
       <c r="B144">
-        <v>1708</v>
+        <v>7424</v>
       </c>
       <c r="C144">
         <v>5259</v>
       </c>
       <c r="D144">
-        <v>7424</v>
+        <v>1708</v>
       </c>
       <c r="E144">
         <v>3270</v>
@@ -12409,13 +12409,13 @@
         <v>9601</v>
       </c>
       <c r="B145">
-        <v>2448</v>
+        <v>9675</v>
       </c>
       <c r="C145">
         <v>5374</v>
       </c>
       <c r="D145">
-        <v>9675</v>
+        <v>2448</v>
       </c>
       <c r="E145">
         <v>3663</v>
@@ -12504,13 +12504,13 @@
         <v>9244</v>
       </c>
       <c r="B146">
-        <v>3037</v>
+        <v>11692</v>
       </c>
       <c r="C146">
         <v>6280</v>
       </c>
       <c r="D146">
-        <v>11692</v>
+        <v>3037</v>
       </c>
       <c r="E146">
         <v>3797</v>
@@ -12599,13 +12599,13 @@
         <v>9243</v>
       </c>
       <c r="B147">
-        <v>2475</v>
+        <v>9773</v>
       </c>
       <c r="C147">
         <v>5826</v>
       </c>
       <c r="D147">
-        <v>9773</v>
+        <v>2475</v>
       </c>
       <c r="E147">
         <v>3235</v>
@@ -12694,13 +12694,13 @@
         <v>11577</v>
       </c>
       <c r="B148">
-        <v>2925</v>
+        <v>11324</v>
       </c>
       <c r="C148">
         <v>6065</v>
       </c>
       <c r="D148">
-        <v>11324</v>
+        <v>2925</v>
       </c>
       <c r="E148">
         <v>3238</v>
@@ -12789,13 +12789,13 @@
         <v>11138</v>
       </c>
       <c r="B149">
-        <v>3271</v>
+        <v>12515</v>
       </c>
       <c r="C149">
         <v>9377</v>
       </c>
       <c r="D149">
-        <v>12515</v>
+        <v>3271</v>
       </c>
       <c r="E149">
         <v>2983</v>
@@ -12884,13 +12884,13 @@
         <v>6276</v>
       </c>
       <c r="B150">
-        <v>3106</v>
+        <v>11273</v>
       </c>
       <c r="C150">
         <v>9900</v>
       </c>
       <c r="D150">
-        <v>11273</v>
+        <v>3106</v>
       </c>
       <c r="E150">
         <v>2362</v>
@@ -12979,13 +12979,13 @@
         <v>13450</v>
       </c>
       <c r="B151">
-        <v>3849</v>
+        <v>13443</v>
       </c>
       <c r="C151">
         <v>8293</v>
       </c>
       <c r="D151">
-        <v>13443</v>
+        <v>3849</v>
       </c>
       <c r="E151">
         <v>2889</v>
@@ -13074,13 +13074,13 @@
         <v>9977</v>
       </c>
       <c r="B152">
-        <v>4862</v>
+        <v>10695</v>
       </c>
       <c r="C152">
         <v>7883</v>
       </c>
       <c r="D152">
-        <v>10695</v>
+        <v>4862</v>
       </c>
       <c r="E152">
         <v>3729</v>
@@ -13169,13 +13169,13 @@
         <v>10952</v>
       </c>
       <c r="B153">
-        <v>4716</v>
+        <v>12567</v>
       </c>
       <c r="C153">
         <v>8963</v>
       </c>
       <c r="D153">
-        <v>12567</v>
+        <v>4716</v>
       </c>
       <c r="E153">
         <v>3291</v>
@@ -13264,13 +13264,13 @@
         <v>10677</v>
       </c>
       <c r="B154">
-        <v>3852</v>
+        <v>13908</v>
       </c>
       <c r="C154">
         <v>9167</v>
       </c>
       <c r="D154">
-        <v>13908</v>
+        <v>3852</v>
       </c>
       <c r="E154">
         <v>3185</v>
@@ -13359,13 +13359,13 @@
         <v>8971</v>
       </c>
       <c r="B155">
-        <v>2370</v>
+        <v>12372</v>
       </c>
       <c r="C155">
         <v>6128</v>
       </c>
       <c r="D155">
-        <v>12372</v>
+        <v>2370</v>
       </c>
       <c r="E155">
         <v>1888</v>
@@ -13454,13 +13454,13 @@
         <v>6554</v>
       </c>
       <c r="B156">
-        <v>2720</v>
+        <v>12786</v>
       </c>
       <c r="C156">
         <v>4586</v>
       </c>
       <c r="D156">
-        <v>12786</v>
+        <v>2720</v>
       </c>
       <c r="E156">
         <v>2833</v>
@@ -13549,13 +13549,13 @@
         <v>7754</v>
       </c>
       <c r="B157">
-        <v>1583</v>
+        <v>12007</v>
       </c>
       <c r="C157">
         <v>5230</v>
       </c>
       <c r="D157">
-        <v>12007</v>
+        <v>1583</v>
       </c>
       <c r="E157">
         <v>3201</v>
@@ -13644,13 +13644,13 @@
         <v>6264</v>
       </c>
       <c r="B158">
-        <v>1301</v>
+        <v>12493</v>
       </c>
       <c r="C158">
         <v>4037</v>
       </c>
       <c r="D158">
-        <v>12493</v>
+        <v>1301</v>
       </c>
       <c r="E158">
         <v>3574</v>
@@ -13739,13 +13739,13 @@
         <v>6228</v>
       </c>
       <c r="B159">
-        <v>1977</v>
+        <v>8924</v>
       </c>
       <c r="C159">
         <v>4902</v>
       </c>
       <c r="D159">
-        <v>8924</v>
+        <v>1977</v>
       </c>
       <c r="E159">
         <v>2388</v>
@@ -13834,13 +13834,13 @@
         <v>8058</v>
       </c>
       <c r="B160">
-        <v>3290</v>
+        <v>12955</v>
       </c>
       <c r="C160">
         <v>6072</v>
       </c>
       <c r="D160">
-        <v>12955</v>
+        <v>3290</v>
       </c>
       <c r="E160">
         <v>3834</v>
@@ -13929,13 +13929,13 @@
         <v>10745</v>
       </c>
       <c r="B161">
-        <v>3577</v>
+        <v>13279</v>
       </c>
       <c r="C161">
         <v>8244</v>
       </c>
       <c r="D161">
-        <v>13279</v>
+        <v>3577</v>
       </c>
       <c r="E161">
         <v>2693</v>
@@ -14024,13 +14024,13 @@
         <v>8186</v>
       </c>
       <c r="B162">
-        <v>3285</v>
+        <v>13762</v>
       </c>
       <c r="C162">
         <v>6016</v>
       </c>
       <c r="D162">
-        <v>13762</v>
+        <v>3285</v>
       </c>
       <c r="E162">
         <v>2700</v>
@@ -14119,13 +14119,13 @@
         <v>14531</v>
       </c>
       <c r="B163">
-        <v>4157</v>
+        <v>17149</v>
       </c>
       <c r="C163">
         <v>6073</v>
       </c>
       <c r="D163">
-        <v>17149</v>
+        <v>4157</v>
       </c>
       <c r="E163">
         <v>2337</v>
@@ -14214,13 +14214,13 @@
         <v>10606</v>
       </c>
       <c r="B164">
-        <v>5112</v>
+        <v>16072</v>
       </c>
       <c r="C164">
         <v>7340</v>
       </c>
       <c r="D164">
-        <v>16072</v>
+        <v>5112</v>
       </c>
       <c r="E164">
         <v>4403</v>
@@ -14309,13 +14309,13 @@
         <v>13107</v>
       </c>
       <c r="B165">
-        <v>2630</v>
+        <v>17063</v>
       </c>
       <c r="C165">
         <v>6912</v>
       </c>
       <c r="D165">
-        <v>17063</v>
+        <v>2630</v>
       </c>
       <c r="E165">
         <v>3224</v>
@@ -14404,13 +14404,13 @@
         <v>7683</v>
       </c>
       <c r="B166">
-        <v>3486</v>
+        <v>16218</v>
       </c>
       <c r="C166">
         <v>7426</v>
       </c>
       <c r="D166">
-        <v>16218</v>
+        <v>3486</v>
       </c>
       <c r="E166">
         <v>2794</v>
@@ -14499,13 +14499,13 @@
         <v>7865</v>
       </c>
       <c r="B167">
-        <v>2408</v>
+        <v>11329</v>
       </c>
       <c r="C167">
         <v>6130</v>
       </c>
       <c r="D167">
-        <v>11329</v>
+        <v>2408</v>
       </c>
       <c r="E167">
         <v>2125</v>
@@ -14593,11 +14593,11 @@
       <c r="A168">
         <v>6044</v>
       </c>
-      <c r="B168">
-        <v>3547</v>
-      </c>
       <c r="C168">
         <v>4159</v>
+      </c>
+      <c r="D168">
+        <v>3547</v>
       </c>
       <c r="E168">
         <v>3651</v>
@@ -14685,11 +14685,11 @@
       <c r="A169">
         <v>7280</v>
       </c>
-      <c r="B169">
-        <v>3145</v>
-      </c>
       <c r="C169">
         <v>4504</v>
+      </c>
+      <c r="D169">
+        <v>3145</v>
       </c>
       <c r="E169">
         <v>3182</v>
@@ -14774,11 +14774,11 @@
       <c r="A170">
         <v>6215</v>
       </c>
-      <c r="B170">
-        <v>1341</v>
-      </c>
       <c r="C170">
         <v>4858</v>
+      </c>
+      <c r="D170">
+        <v>1341</v>
       </c>
       <c r="E170">
         <v>2351</v>
@@ -14860,11 +14860,11 @@
       <c r="A171">
         <v>7421</v>
       </c>
-      <c r="B171">
-        <v>1282</v>
-      </c>
       <c r="C171">
         <v>5909</v>
+      </c>
+      <c r="D171">
+        <v>1282</v>
       </c>
       <c r="E171">
         <v>3931</v>
@@ -14943,7 +14943,7 @@
       <c r="A172">
         <v>11349</v>
       </c>
-      <c r="B172">
+      <c r="D172">
         <v>1849</v>
       </c>
       <c r="F172">
@@ -15020,7 +15020,7 @@
       <c r="A173">
         <v>9479</v>
       </c>
-      <c r="B173">
+      <c r="D173">
         <v>1409</v>
       </c>
       <c r="F173">

</xml_diff>